<commit_message>
POST Method and Plan div added
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7770" activeTab="3"/>
+    <workbookView windowWidth="19485" windowHeight="7770" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Todo:</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t>https://app.diagrams.net/#G1wKTWF5907AMjdvuFrYsDYcYMQ8MhcJ8H</t>
+  </si>
+  <si>
+    <t>Learning topics:</t>
+  </si>
+  <si>
+    <t>MVT Architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middlewares </t>
+  </si>
+  <si>
+    <t>Jinja Template</t>
+  </si>
+  <si>
+    <t>Design Patterns</t>
   </si>
 </sst>
 </file>
@@ -148,10 +163,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -177,16 +192,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,8 +222,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -210,7 +263,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,7 +271,36 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,30 +322,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -276,50 +335,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -336,31 +351,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,7 +429,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,139 +525,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,6 +556,21 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -569,17 +599,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -616,17 +642,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -647,148 +662,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1164,7 +1179,7 @@
   <sheetPr/>
   <dimension ref="A2:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:A49"/>
     </sheetView>
   </sheetViews>
@@ -1361,7 +1376,7 @@
   <sheetPr/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1446,15 +1461,15 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="14.75" customWidth="1"/>
     <col min="2" max="2" width="67.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1464,6 +1479,31 @@
       </c>
       <c r="B1" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>